<commit_message>
update: draw figures in R
</commit_message>
<xml_diff>
--- a/data-result/data-envs.xlsx
+++ b/data-result/data-envs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wyw/Documents/Chaper2/github-code/segmentation-3D/data-result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D632FECE-A1F8-3A4E-8DC8-32DCD5D5CB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B61BD3-2393-774C-89FF-F0B3CF8418D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14120" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="149">
   <si>
     <t>plan</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>time</t>
-  </si>
-  <si>
-    <t>max-illumiantion</t>
   </si>
   <si>
     <t>min-illumiantion</t>
@@ -491,13 +488,21 @@
   <si>
     <t>8-5</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max-illumiantion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +529,11 @@
       <name val="TimesNewRomanPSMT"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPSMT"/>
     </font>
   </fonts>
   <fills count="2">
@@ -561,24 +571,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -881,18 +896,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="131" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -903,62 +920,66 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="D3">
         <v>56</v>
@@ -976,18 +997,21 @@
         <v>3.1</v>
       </c>
       <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
       <c r="D4">
         <v>55.6</v>
@@ -1005,18 +1029,21 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
       </c>
       <c r="D5">
         <v>57.4</v>
@@ -1034,18 +1061,21 @@
         <v>5.5</v>
       </c>
       <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6">
         <v>56</v>
@@ -1063,18 +1093,21 @@
         <v>5.4</v>
       </c>
       <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
       </c>
       <c r="D7">
         <v>54.7</v>
@@ -1092,18 +1125,21 @@
         <v>0.3</v>
       </c>
       <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
       </c>
       <c r="D8">
         <v>54.5</v>
@@ -1121,18 +1157,21 @@
         <v>0.1</v>
       </c>
       <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
       </c>
       <c r="D9">
         <v>52.8</v>
@@ -1150,18 +1189,21 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="I9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
       </c>
       <c r="D10">
         <v>55</v>
@@ -1179,18 +1221,21 @@
         <v>6.6</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
       </c>
       <c r="D11">
         <v>55.6</v>
@@ -1208,18 +1253,21 @@
         <v>3.9</v>
       </c>
       <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>54</v>
       </c>
       <c r="D12">
         <v>55.3</v>
@@ -1237,18 +1285,21 @@
         <v>3.3</v>
       </c>
       <c r="I12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
       </c>
       <c r="D13">
         <v>51</v>
@@ -1266,18 +1317,21 @@
         <v>0.3</v>
       </c>
       <c r="I13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>60</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>61</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
       </c>
       <c r="D14">
         <v>51.1</v>
@@ -1295,18 +1349,21 @@
         <v>0.5</v>
       </c>
       <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>66</v>
       </c>
       <c r="D15">
         <v>48.6</v>
@@ -1324,18 +1381,21 @@
         <v>2.7</v>
       </c>
       <c r="I15" t="s">
+        <v>66</v>
+      </c>
+      <c r="J15" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>68</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" t="s">
-        <v>70</v>
       </c>
       <c r="D16">
         <v>47.7</v>
@@ -1353,18 +1413,21 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>73</v>
-      </c>
-      <c r="C17" t="s">
-        <v>74</v>
       </c>
       <c r="D17">
         <v>49.5</v>
@@ -1382,18 +1445,21 @@
         <v>4</v>
       </c>
       <c r="I17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>76</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>78</v>
       </c>
       <c r="D18">
         <v>46.8</v>
@@ -1411,18 +1477,21 @@
         <v>1.8</v>
       </c>
       <c r="I18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
       </c>
       <c r="D19">
         <v>50.2</v>
@@ -1440,18 +1509,21 @@
         <v>0.1</v>
       </c>
       <c r="I19" t="s">
+        <v>82</v>
+      </c>
+      <c r="J19" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>84</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>85</v>
-      </c>
-      <c r="C20" t="s">
-        <v>86</v>
       </c>
       <c r="D20">
         <v>49.8</v>
@@ -1469,18 +1541,21 @@
         <v>0.4</v>
       </c>
       <c r="I20" t="s">
+        <v>86</v>
+      </c>
+      <c r="J20" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>88</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
       </c>
       <c r="D21">
         <v>37.799999999999997</v>
@@ -1498,18 +1573,21 @@
         <v>3.1</v>
       </c>
       <c r="I21" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>92</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>93</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
       </c>
       <c r="D22">
         <v>36.6</v>
@@ -1527,18 +1605,21 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J22" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>96</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>97</v>
-      </c>
-      <c r="C23" t="s">
-        <v>98</v>
       </c>
       <c r="D23">
         <v>45.8</v>
@@ -1556,18 +1637,21 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>102</v>
       </c>
       <c r="D24">
         <v>45.4</v>
@@ -1585,18 +1669,21 @@
         <v>1.5</v>
       </c>
       <c r="I24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>104</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>105</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
       </c>
       <c r="D25">
         <v>44.7</v>
@@ -1614,18 +1701,21 @@
         <v>2.9</v>
       </c>
       <c r="I25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>108</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>109</v>
-      </c>
-      <c r="C26" t="s">
-        <v>110</v>
       </c>
       <c r="D26">
         <v>45.6</v>
@@ -1643,18 +1733,21 @@
         <v>4.3</v>
       </c>
       <c r="I26" t="s">
+        <v>110</v>
+      </c>
+      <c r="J26" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>112</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>113</v>
-      </c>
-      <c r="C27" t="s">
-        <v>114</v>
       </c>
       <c r="D27">
         <v>36.5</v>
@@ -1672,18 +1765,21 @@
         <v>2.1</v>
       </c>
       <c r="I27" t="s">
+        <v>114</v>
+      </c>
+      <c r="J27" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>116</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>117</v>
-      </c>
-      <c r="C28" t="s">
-        <v>118</v>
       </c>
       <c r="D28">
         <v>35.799999999999997</v>
@@ -1701,18 +1797,21 @@
         <v>2.9</v>
       </c>
       <c r="I28" t="s">
+        <v>118</v>
+      </c>
+      <c r="J28" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>120</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>121</v>
-      </c>
-      <c r="C29" t="s">
-        <v>122</v>
       </c>
       <c r="D29">
         <v>44.5</v>
@@ -1730,18 +1829,21 @@
         <v>1.6</v>
       </c>
       <c r="I29" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>124</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>125</v>
-      </c>
-      <c r="C30" t="s">
-        <v>126</v>
       </c>
       <c r="D30">
         <v>43.2</v>
@@ -1759,18 +1861,21 @@
         <v>0.7</v>
       </c>
       <c r="I30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>128</v>
       </c>
-      <c r="B31" t="s">
-        <v>129</v>
-      </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>43.9</v>
@@ -1788,18 +1893,21 @@
         <v>0.9</v>
       </c>
       <c r="I31" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>131</v>
       </c>
-      <c r="B32" t="s">
-        <v>132</v>
-      </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32">
         <v>43.4</v>
@@ -1817,15 +1925,18 @@
         <v>3.3</v>
       </c>
       <c r="I32" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="15">
+        <v>132</v>
+      </c>
+      <c r="J32" s="7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15">
       <c r="A33" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C33" s="4">
         <v>0.7895833333333333</v>
@@ -1836,22 +1947,27 @@
       <c r="E33" s="5">
         <v>0</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5">
+        <v>0.2</v>
+      </c>
       <c r="G33" s="5">
         <v>52</v>
       </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="6" t="str">
+      <c r="I33" t="str">
         <f>CONCATENATE(B33,"_",A33)</f>
         <v>15-3_31-81</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15">
+      <c r="J33" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15">
       <c r="A34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C34" s="4">
         <v>0.79027777777777775</v>
@@ -1862,22 +1978,27 @@
       <c r="E34" s="5">
         <v>0</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="5">
+        <v>0.2</v>
+      </c>
       <c r="G34" s="5">
         <v>52</v>
       </c>
       <c r="H34" s="5"/>
-      <c r="I34" s="6" t="str">
+      <c r="I34" t="str">
         <f t="shared" ref="I34:I38" si="0">CONCATENATE(B34,"_",A34)</f>
         <v>15-5_31-82</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15">
+      <c r="J34" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15">
       <c r="A35" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C35" s="4">
         <v>0.79166666666666663</v>
@@ -1888,22 +2009,27 @@
       <c r="E35" s="5">
         <v>0</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="5">
+        <v>0.1</v>
+      </c>
       <c r="G35" s="5">
         <v>52</v>
       </c>
       <c r="H35" s="5"/>
-      <c r="I35" s="6" t="str">
+      <c r="I35" t="str">
         <f t="shared" si="0"/>
         <v>10-3_31-83</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15">
+      <c r="J35" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15">
       <c r="A36" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C36" s="4">
         <v>0.79305555555555562</v>
@@ -1915,23 +2041,26 @@
         <v>0</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G36" s="5">
         <v>52</v>
       </c>
       <c r="H36" s="5"/>
-      <c r="I36" s="6" t="str">
+      <c r="I36" t="str">
         <f t="shared" si="0"/>
         <v>10-5_31-84</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15">
+      <c r="J36" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15">
       <c r="A37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C37" s="4">
         <v>0.7944444444444444</v>
@@ -1945,19 +2074,24 @@
       <c r="F37" s="5">
         <v>0</v>
       </c>
-      <c r="G37" s="5"/>
+      <c r="G37" s="5">
+        <v>52</v>
+      </c>
       <c r="H37" s="5"/>
-      <c r="I37" s="6" t="str">
+      <c r="I37" t="str">
         <f t="shared" si="0"/>
         <v>8-3_31-85</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15">
+      <c r="J37" s="7">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15">
       <c r="A38" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C38" s="4">
         <v>0.79583333333333339</v>
@@ -1969,13 +2103,18 @@
         <v>0</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" s="5"/>
+        <v>134</v>
+      </c>
+      <c r="G38" s="5">
+        <v>52</v>
+      </c>
       <c r="H38" s="5"/>
-      <c r="I38" s="6" t="str">
+      <c r="I38" t="str">
         <f t="shared" si="0"/>
         <v>8-5_31-86</v>
+      </c>
+      <c r="J38" s="7">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>